<commit_message>
Atualizada lista de comp.
</commit_message>
<xml_diff>
--- a/Hardware/pcb_universal/Lista_comp/Lista_de_Componentes_Acionamento.xlsx
+++ b/Hardware/pcb_universal/Lista_comp/Lista_de_Componentes_Acionamento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7785"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Qtd</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>Barra pino femea simples</t>
+  </si>
+  <si>
+    <t>5KΩ</t>
+  </si>
+  <si>
+    <t>Potenciômetro</t>
+  </si>
+  <si>
+    <t>PTH 5mm</t>
+  </si>
+  <si>
+    <t>LDR 5mm</t>
+  </si>
+  <si>
+    <t>10KΩ</t>
+  </si>
+  <si>
+    <t>NRF24l01</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>OU</t>
   </si>
 </sst>
 </file>
@@ -488,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:J22"/>
+  <dimension ref="A4:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,11 +843,21 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -831,15 +865,84 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
atualizado a lista de comp.
</commit_message>
<xml_diff>
--- a/Hardware/pcb_universal/Lista_comp/Lista_de_Componentes_Acionamento.xlsx
+++ b/Hardware/pcb_universal/Lista_comp/Lista_de_Componentes_Acionamento.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7785"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Qtd</t>
   </si>
@@ -183,6 +183,26 @@
   </si>
   <si>
     <t>OU</t>
+  </si>
+  <si>
+    <r>
+      <t>220</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>220Ω</t>
+  </si>
+  <si>
+    <t>360Ω</t>
   </si>
 </sst>
 </file>
@@ -512,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:J28"/>
+  <dimension ref="A4:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +633,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -624,7 +644,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -633,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -644,16 +664,16 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -664,16 +684,16 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -684,16 +704,16 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -704,16 +724,16 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -724,16 +744,16 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -744,16 +764,16 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -764,16 +784,16 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -784,16 +804,16 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -804,13 +824,13 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>6</v>
@@ -827,10 +847,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>6</v>
@@ -847,17 +867,15 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -869,13 +887,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -892,11 +910,16 @@
         <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -907,35 +930,71 @@
         <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -944,6 +1003,27 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>